<commit_message>
Fix product scratch code on main page
</commit_message>
<xml_diff>
--- a/DoAnNhom/books.xlsx
+++ b/DoAnNhom/books.xlsx
@@ -494,7 +494,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Lén Nhặt Chuyện Đời</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>42500</t>
@@ -502,7 +506,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/len-nhat-chuyen-doi-404720.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/len-nhat-chuyen-doi-404720.html</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -562,7 +566,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Trắng</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>79000</t>
@@ -570,7 +578,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/trang-tac-gia-han-kang.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/trang-tac-gia-han-kang.html</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -630,7 +638,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cây Cam Ngọt Của Tôi</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>88560</t>
@@ -638,7 +650,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/cay-cam-ngot-cua-toi.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/cay-cam-ngot-cua-toi.html</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -698,7 +710,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Trường Ca Achilles</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>127920</t>
@@ -706,7 +722,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/truong-ca-achilles.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/truong-ca-achilles.html</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -766,7 +782,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Nhà Giả Kim (Tái Bản 2020)</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>64780</t>
@@ -774,7 +794,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/nha-gia-kim-tai-ban-2020.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/nha-gia-kim-tai-ban-2020.html</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -834,7 +854,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Người Đàn Ông Mang Tên OVE (Tái Bản)</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>134400</t>
@@ -842,7 +866,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/nguoi-dan-ong-mang-ten-ove-tai-ban.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/nguoi-dan-ong-mang-ten-ove-tai-ban.html</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -902,7 +926,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ngày Xưa Có Một Chuyện Tình (Tái Bản 2019)</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>105000</t>
@@ -910,7 +938,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/ngay-xua-co-mot-chuyen-tinh-tai-ban-2019.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/ngay-xua-co-mot-chuyen-tinh-tai-ban-2019.html</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -970,7 +998,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25 Độ Âm</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>129560</t>
@@ -978,7 +1010,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/25-do-am.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/25-do-am.html</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1038,7 +1070,11 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sưởi Ấm Mặt Trời - Phần Tiếp Theo Của Cây Cam Ngọt Của Tôi</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>128000</t>
@@ -1046,7 +1082,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/suoi-am-mat-troi-phan-tiep-theo-cua-cay-cam-ngot-cua-toi.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/suoi-am-mat-troi-phan-tiep-theo-cua-cay-cam-ngot-cua-toi.html</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1106,7 +1142,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ngày Xưa Có Một Chuyện Tình - Khổ Thường - Bìa Hồng - Tặng Kèm Poster Hình Ảnh Phim Và Postcard Hình Ảnh Phim</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>110700</t>
@@ -1114,7 +1154,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.fahasa.com/ngay-xua-co-mot-chuyen-tinh-kho-thuong-bia-hong-tang-kem-poster-hinh-anh-phim-va-postcard-hinh-anh-phim.html?fhs_campaign=CATEGORY</t>
+          <t>https://www.fahasa.com/ngay-xua-co-mot-chuyen-tinh-kho-thuong-bia-hong-tang-kem-poster-hinh-anh-phim-va-postcard-hinh-anh-phim.html</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">

</xml_diff>